<commit_message>
Interfaz de archivos lista
</commit_message>
<xml_diff>
--- a/tabla1.xlsx
+++ b/tabla1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevUser\Desktop\GeneradorReporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E792E7-EC46-4DEC-98F5-86131F698427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7CA310-0061-4A29-9EE8-BB18AAE41280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,65 +337,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras en la parte de la interfaz
</commit_message>
<xml_diff>
--- a/tabla1.xlsx
+++ b/tabla1.xlsx
@@ -8,20 +8,73 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevUser\Desktop\GeneradorReporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7CA310-0061-4A29-9EE8-BB18AAE41280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB6F88A-7C86-4A62-A62E-0A5FD3112F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -339,7 +392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -774,4 +827,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D8E5E8-2FC7-4E7F-A432-E932121E56B7}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>